<commit_message>
Added Camera to layout diagram
</commit_message>
<xml_diff>
--- a/docs/Preliminary Design/BOM.xlsx
+++ b/docs/Preliminary Design/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\their\Documents\THONNY\ME405\me405bin9\TermProj\docs\Preliminary Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\their\Documents\THONNY\ME405\me405bin9\TermProj\TermProject\docs\Preliminary Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3926EA8E-968A-4A2F-A075-FA836E190656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA16755E-7411-46F1-BD1C-55FB6659D002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Part Number</t>
   </si>
@@ -131,13 +131,28 @@
     <t>https://outofdarts.com/products/micro-switch-1a-for-mosfet-builds</t>
   </si>
   <si>
-    <t>https://www.andymark.com/products/245-rpm-12v-gearmotor-with-2-channel-encoder</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
-    <t>245 RPM 12V Gear Motor with Encoder</t>
+    <t>OutOfDarts</t>
+  </si>
+  <si>
+    <t>Polulu</t>
+  </si>
+  <si>
+    <t>12V 50:1 Metal Gearmotor with Encoder</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/4753/resources</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Deep Groove Ball Bearing 80x100x10mm</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-6816-2RS-Bearing-80x100x10mm-Bearings/dp/B07RQ4RXDR/ref=sr_1_2_sspa?crid=245V7BXKB1Z1W&amp;keywords=large%2Bbearing&amp;qid=1706830027&amp;sprefix=large%2Bbearing%2Caps%2C144&amp;sr=8-2-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -145,7 +160,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -322,7 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -336,6 +351,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -354,8 +374,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -640,7 +661,7 @@
   <dimension ref="B3:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -655,24 +676,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="6" spans="2:8" ht="51.75" customHeight="1" thickBot="1">
       <c r="B6" s="4" t="s">
@@ -698,205 +719,233 @@
       </c>
     </row>
     <row r="8" spans="2:8">
+      <c r="B8" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="6">
         <v>8.5</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="6">
         <f>F8*G8</f>
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:8">
+      <c r="B9" s="14"/>
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="6">
         <v>9</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="6">
         <f>F9*G9</f>
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:8">
+      <c r="B10" s="14"/>
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="6">
         <v>9</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="6">
         <f t="shared" ref="H10:H12" si="0">F10*G10</f>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:8">
+      <c r="B11" s="14"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="6">
         <v>6</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:8">
+      <c r="B12" s="14"/>
       <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="6">
         <v>0.8</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="6">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:8">
+      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" s="12">
-        <v>19</v>
-      </c>
-      <c r="H15" s="12">
-        <f t="shared" ref="H15" si="1">F15*G15</f>
-        <v>19</v>
+      <c r="G15" s="6">
+        <v>51.95</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" ref="H15:H17" si="1">F15*G15</f>
+        <v>51.95</v>
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="7:8">
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="7:8">
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="7:8">
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="7:8">
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="7:8">
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="7:8">
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="7:8">
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="7:8">
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="7:8">
-      <c r="G25" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="12">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>13.99</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="1"/>
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="G25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="6">
         <f>SUM(H8:H23)</f>
-        <v>61.6</v>
-      </c>
-    </row>
-    <row r="26" spans="7:8">
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="7:8">
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="7:8">
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="7:8">
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-    </row>
-    <row r="30" spans="7:8">
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="7:8">
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="7:8">
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+        <v>108.54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="7:8">
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="7:8">
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:H4"/>
+    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E8" r:id="rId1" xr:uid="{E76B369B-57F1-426B-9490-EE3B5C49D4BC}"/>
@@ -904,7 +953,7 @@
     <hyperlink ref="E10" r:id="rId3" xr:uid="{D5C3F60D-7AC8-40DC-A385-9E6E42A0A4FD}"/>
     <hyperlink ref="E11" r:id="rId4" xr:uid="{36042352-E2AE-4E42-B4C8-D751BEF0D595}"/>
     <hyperlink ref="E12" r:id="rId5" xr:uid="{A351857F-B20E-47A5-9D4E-239E0F0C62F9}"/>
-    <hyperlink ref="E15" r:id="rId6" xr:uid="{90975FEC-B0E2-45C0-A565-C79C05F45B7F}"/>
+    <hyperlink ref="E17" r:id="rId6" xr:uid="{DBFF3B4C-1A79-4B54-A71A-5470D9A0ACFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>